<commit_message>
Add read_excel helper method
</commit_message>
<xml_diff>
--- a/tests/input/2kp50.xlsx
+++ b/tests/input/2kp50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B243DF72-224B-45A7-8042-7F90B8722166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BC72FF-A24C-4F3D-8D0F-A910EAC8C8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3555" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
+    <workbookView xWindow="5010" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="2" r:id="rId1"/>
@@ -35,10 +35,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1426,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D21B3-32B4-4C12-A7C7-63C45A248C7B}">
   <dimension ref="A1:RY2"/>
   <sheetViews>
-    <sheetView topLeftCell="RF1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:RY1"/>
+    <sheetView topLeftCell="RE1" workbookViewId="0">
+      <selection activeCell="RL4" sqref="RL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,10 +4394,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72422ABD-857E-4B13-A4DD-3030381878EF}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,10 +4437,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="C4">
-        <v>1531</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4452,10 +4448,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="C5">
-        <v>1577</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,10 +4459,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2087</v>
+        <v>2079</v>
       </c>
       <c r="C6">
-        <v>1588</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4474,10 +4470,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2079</v>
+        <v>2075</v>
       </c>
       <c r="C7">
-        <v>1589</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4485,10 +4481,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2075</v>
+        <v>2070</v>
       </c>
       <c r="C8">
-        <v>1635</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4496,10 +4492,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2070</v>
+        <v>2062</v>
       </c>
       <c r="C9">
-        <v>1636</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4507,10 +4503,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="C10">
-        <v>1662</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4518,10 +4514,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2059</v>
+        <v>2038</v>
       </c>
       <c r="C11">
-        <v>1694</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4529,10 +4525,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2038</v>
+        <v>2029</v>
       </c>
       <c r="C12">
-        <v>1708</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4540,10 +4536,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C13">
-        <v>1715</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4551,10 +4547,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2028</v>
+        <v>2015</v>
       </c>
       <c r="C14">
-        <v>1716</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4562,10 +4558,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="C15">
-        <v>1730</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,10 +4569,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="C16">
-        <v>1735</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4584,10 +4580,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2003</v>
+        <v>1993</v>
       </c>
       <c r="C17">
-        <v>1755</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4595,10 +4591,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2003</v>
+        <v>1987</v>
       </c>
       <c r="C18">
-        <v>1755</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4606,10 +4602,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1993</v>
+        <v>1982</v>
       </c>
       <c r="C19">
-        <v>1761</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4617,10 +4613,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1987</v>
+        <v>1975</v>
       </c>
       <c r="C20">
-        <v>1769</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,10 +4624,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1982</v>
+        <v>1973</v>
       </c>
       <c r="C21">
-        <v>1772</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4639,10 +4635,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1975</v>
+        <v>1956</v>
       </c>
       <c r="C22">
-        <v>1773</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4650,10 +4646,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1973</v>
+        <v>1931</v>
       </c>
       <c r="C23">
-        <v>1808</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4661,10 +4657,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1956</v>
+        <v>1893</v>
       </c>
       <c r="C24">
-        <v>1827</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4672,10 +4668,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1931</v>
+        <v>1862</v>
       </c>
       <c r="C25">
-        <v>1857</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4683,10 +4679,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1893</v>
+        <v>1830</v>
       </c>
       <c r="C26">
-        <v>1902</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4694,10 +4690,10 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1862</v>
+        <v>1826</v>
       </c>
       <c r="C27">
-        <v>1909</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -4705,10 +4701,10 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1830</v>
+        <v>1822</v>
       </c>
       <c r="C28">
-        <v>1914</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -4716,10 +4712,10 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1826</v>
+        <v>1814</v>
       </c>
       <c r="C29">
-        <v>1917</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -4727,10 +4723,10 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1822</v>
+        <v>1783</v>
       </c>
       <c r="C30">
-        <v>1929</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4738,10 +4734,10 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1814</v>
+        <v>1755</v>
       </c>
       <c r="C31">
-        <v>1949</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4749,10 +4745,10 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1783</v>
+        <v>1742</v>
       </c>
       <c r="C32">
-        <v>1965</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4760,10 +4756,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1755</v>
+        <v>1711</v>
       </c>
       <c r="C33">
-        <v>1969</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -4771,10 +4767,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1742</v>
+        <v>1639</v>
       </c>
       <c r="C34">
-        <v>1986</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4782,10 +4778,10 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1711</v>
+        <v>1636</v>
       </c>
       <c r="C35">
-        <v>2002</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4793,42 +4789,9 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1639</v>
+        <v>1547</v>
       </c>
       <c r="C36">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>1636</v>
-      </c>
-      <c r="C37">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>1547</v>
-      </c>
-      <c r="C38">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>1547</v>
-      </c>
-      <c r="C39">
         <v>2020</v>
       </c>
     </row>

</xml_diff>